<commit_message>
back end code modifications to filter products
</commit_message>
<xml_diff>
--- a/anotherdb.xlsx
+++ b/anotherdb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raana\Desktop\Embryolisse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raana\Desktop\Embryolisse\embryorepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1662FA00-3ABA-4666-AB5E-9B490EB06632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7906512-1E79-4DDC-A0AC-6F3072BA93C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -201,9 +198,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>temp</t>
-  </si>
-  <si>
     <t>breakouts</t>
   </si>
   <si>
@@ -244,6 +238,171 @@
   </si>
   <si>
     <t>dry, normal, sensitive</t>
+  </si>
+  <si>
+    <t>dark spots, dryness, uneven texture</t>
+  </si>
+  <si>
+    <t>dryness</t>
+  </si>
+  <si>
+    <t>The “must-have” 6-in-1 multi-function nourishing moisturizer</t>
+  </si>
+  <si>
+    <t>A Vitamin-Infused Powerhouse for Radiant Skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active hydration for radiantly beautiful skin. </t>
+  </si>
+  <si>
+    <t>sometimes, frequently</t>
+  </si>
+  <si>
+    <t>oily, combination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ultimate in anti‑blemish skincare </t>
+  </si>
+  <si>
+    <t>face</t>
+  </si>
+  <si>
+    <t>acne, oiliness, redness</t>
+  </si>
+  <si>
+    <t>Nourishing repair cream with Shea Butter</t>
+  </si>
+  <si>
+    <t>dry</t>
+  </si>
+  <si>
+    <t>hands</t>
+  </si>
+  <si>
+    <t>dry, sensitive</t>
+  </si>
+  <si>
+    <t>This cream changes the life of dry and sensitive skin</t>
+  </si>
+  <si>
+    <t>The best of the coconut in a water-free powder</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>oiliness</t>
+  </si>
+  <si>
+    <t>The Foaming Cream-Milk has a rich and creamy nourishing texture</t>
+  </si>
+  <si>
+    <t>Gentle care with Lemon Caviar</t>
+  </si>
+  <si>
+    <t>dark spots, uneven texture</t>
+  </si>
+  <si>
+    <t>fine lines, wrinkles</t>
+  </si>
+  <si>
+    <t>This mask envelops the skin in a cocoon of softness, leaving a sensation of infinite well-being</t>
+  </si>
+  <si>
+    <t>This vevelty cream enriched in organic kangaroo paw flower plumps the skin daily for continuous correction of wrinkles and firmness</t>
+  </si>
+  <si>
+    <t>Enriched with active plant oils, this dry oil protects and beautifies skin and hair</t>
+  </si>
+  <si>
+    <t>dryness, uneven texture</t>
+  </si>
+  <si>
+    <t>dry, normal</t>
+  </si>
+  <si>
+    <t>Enhance your beauty routine with the New Lait-Crème Fluid+, where natural care meets exceptional performance</t>
+  </si>
+  <si>
+    <t>7-in-1 multi-functional hydrating and nourishing moisturizer</t>
+  </si>
+  <si>
+    <t>sensitive</t>
+  </si>
+  <si>
+    <t>A skincare innovation with French Big Clover extract</t>
+  </si>
+  <si>
+    <t>fine lines, wrinkles, dryness</t>
+  </si>
+  <si>
+    <t>The Winter Dry Skin Essentials curated routine offers the ultimate solution for parched skin, providing hydration and relief for your face, lips, and hands</t>
+  </si>
+  <si>
+    <t>face, lips, hands</t>
+  </si>
+  <si>
+    <t>normal, combination</t>
+  </si>
+  <si>
+    <t>Enriched in white nymphaea and a hyaluronic acid active complex, the Hydra-Cream Light replenishes the skin with water and delivers intense, long-lasting hydration</t>
+  </si>
+  <si>
+    <t>dryness, redness</t>
+  </si>
+  <si>
+    <t>The Smooth-Active Cream is the ideal care for women with a busy lifestyle</t>
+  </si>
+  <si>
+    <t>combination, oily</t>
+  </si>
+  <si>
+    <t>The Anti-Blemish Serum is a powerful treatment that targets and diminishes 6 different types of skin imperfections: acne, redness, breakouts, blackheads, blemishes, and excess oil.</t>
+  </si>
+  <si>
+    <t>Formulated with 98% natural ingredients, vegetable glycerin-enriched Mattifying Moisturizer is perfectly suited as a day—or night-time treatment after the Anti-Blemish Serum</t>
+  </si>
+  <si>
+    <t>acne, oiliness, uneven texture</t>
+  </si>
+  <si>
+    <t>This gel mask, enriched with white nymphaea and hyaluronic acid, instantly replenishes the water reserves of even the thirstiest skin</t>
+  </si>
+  <si>
+    <t>Moisturizes and nourishes, protects and soothes dry and damaged lips with active ingredients of natural origin</t>
+  </si>
+  <si>
+    <t>lips</t>
+  </si>
+  <si>
+    <t>face, body, lips</t>
+  </si>
+  <si>
+    <t>Cicalisse Cream calms and restores the skin’s barrier function while moisturizing the damaged and weakened epidermis</t>
+  </si>
+  <si>
+    <t>A refreshing toner, comprised of 4 organic beneficial floral waters, that can be used as a toner, a refreshing mist or a make-up fixing mist</t>
+  </si>
+  <si>
+    <t>uneven texture</t>
+  </si>
+  <si>
+    <t>face, eyes, lips</t>
+  </si>
+  <si>
+    <t>This 4-in-1 milk cleanses, removes makeup, moisturizes, and soothes all skin types, even sensitive ones</t>
+  </si>
+  <si>
+    <t>A gentle and efficient micellar water that cleanses and removes makeup from the face, eyes, and lips</t>
+  </si>
+  <si>
+    <t>eyes</t>
+  </si>
+  <si>
+    <t>Genuine smoothing eye care, it acts simultaneously on dark circles, under-eye bags and fine lines for a rested, more youthful appearance after 28 days</t>
+  </si>
+  <si>
+    <t>product_id</t>
   </si>
 </sst>
 </file>
@@ -580,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -600,37 +759,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
         <v>62</v>
-      </c>
-      <c r="I1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
@@ -638,34 +797,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -673,16 +832,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -690,13 +867,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -704,13 +902,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -718,13 +937,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -732,13 +972,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -746,13 +1007,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -760,13 +1042,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
@@ -774,13 +1077,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -788,13 +1112,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
@@ -802,13 +1147,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>63</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
@@ -816,13 +1182,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
@@ -830,13 +1217,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" t="s">
+        <v>69</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -844,13 +1252,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" t="s">
+        <v>69</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
@@ -858,13 +1287,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
@@ -872,13 +1322,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" t="s">
+        <v>69</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
@@ -886,13 +1357,34 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" t="s">
+        <v>69</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
@@ -900,13 +1392,34 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" t="s">
+        <v>69</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
@@ -914,13 +1427,34 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" t="s">
+        <v>69</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
@@ -928,13 +1462,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>111</v>
+      </c>
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" t="s">
+        <v>69</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
@@ -942,13 +1497,34 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>113</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" t="s">
+        <v>69</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
@@ -956,13 +1532,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" t="s">
+        <v>69</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
@@ -970,13 +1567,34 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" t="s">
+        <v>69</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
@@ -984,13 +1602,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" t="s">
+        <v>69</v>
+      </c>
+      <c r="J25" t="s">
+        <v>69</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
@@ -998,13 +1637,34 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>121</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" t="s">
+        <v>69</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
@@ -1012,13 +1672,34 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>122</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" t="s">
+        <v>69</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
@@ -1026,13 +1707,34 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>124</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" t="s">
+        <v>63</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>